<commit_message>
New sheet added to excel.
</commit_message>
<xml_diff>
--- a/HieratchialInheritance/src/main/resources/TestData.xlsx
+++ b/HieratchialInheritance/src/main/resources/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrit\git\Inheritance\HieratchialInheritance\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A08A31DD-2F72-4EE0-8355-925137872338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56D837B9-719D-4A5D-9EBE-69CFC10150B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07CFF399-4F12-4017-AADB-82B3462B9FD8}"/>
+    <workbookView xWindow="6900" yWindow="1800" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{07CFF399-4F12-4017-AADB-82B3462B9FD8}"/>
   </bookViews>
   <sheets>
     <sheet name="IDName" sheetId="1" r:id="rId1"/>
+    <sheet name="Marks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>Vashnavi</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Vyshnavi</t>
   </si>
 </sst>
 </file>
@@ -402,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828FA347-2B55-466D-B243-894FC334F64A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +450,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D889ED4C-10DB-44DF-874C-A8E2F50B92B7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>